<commit_message>
Added support for multiple sheets
</commit_message>
<xml_diff>
--- a/test/spreadsheets/excel_mac_2011-basic.xlsx
+++ b/test/spreadsheets/excel_mac_2011-basic.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>One</t>
   </si>
@@ -31,17 +32,39 @@
   </si>
   <si>
     <t>Four</t>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -70,7 +93,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -405,7 +428,7 @@
       <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="10.83203125" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -424,6 +447,42 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="10.83203125" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>